<commit_message>
add Muhammad to list
</commit_message>
<xml_diff>
--- a/Logistics/Rosters.xlsx
+++ b/Logistics/Rosters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpruim/projects/github/JMM2019/Logistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9A7713-7986-F548-BFF6-E31162A42872}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065CA6D8-C51A-B549-BF20-1217DD24385C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15500" activeTab="1" xr2:uid="{AECAB193-3CA1-8242-A385-6889D200F4EB}"/>
+    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15500" activeTab="3" xr2:uid="{AECAB193-3CA1-8242-A385-6889D200F4EB}"/>
   </bookViews>
   <sheets>
     <sheet name="MC2" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="247">
   <si>
     <t>Max</t>
   </si>
@@ -757,13 +757,25 @@
   </si>
   <si>
     <t>C.</t>
+  </si>
+  <si>
+    <t>mali@jhu.edu</t>
+  </si>
+  <si>
+    <t>Muhammad</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Yousuf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -781,6 +793,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -818,12 +836,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1864,11 +1885,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F72D6F-8F28-534C-A98A-B6F7ABB3A10C}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2988,13 +3013,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1470E79-0876-1443-9948-BFC97695843C}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3382,6 +3414,20 @@
       </c>
       <c r="F25" s="2"/>
     </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B26" t="s">
+        <v>245</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D26" t="s">
+        <v>243</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add muhammad to MC2 as well
</commit_message>
<xml_diff>
--- a/Logistics/Rosters.xlsx
+++ b/Logistics/Rosters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpruim/projects/github/JMM2019/Logistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065CA6D8-C51A-B549-BF20-1217DD24385C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DF9527-1F50-8349-893A-D69E2B362A6E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15500" activeTab="3" xr2:uid="{AECAB193-3CA1-8242-A385-6889D200F4EB}"/>
+    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15500" activeTab="1" xr2:uid="{AECAB193-3CA1-8242-A385-6889D200F4EB}"/>
   </bookViews>
   <sheets>
     <sheet name="MC2" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="247">
   <si>
     <t>Max</t>
   </si>
@@ -1161,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E4F9ED-4C0F-9748-94FA-08046731256F}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1876,6 +1876,20 @@
         <v>94</v>
       </c>
     </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B46" t="s">
+        <v>245</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D46" t="s">
+        <v>243</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1883,10 +1897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F72D6F-8F28-534C-A98A-B6F7ABB3A10C}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2282,6 +2296,20 @@
         <v>94</v>
       </c>
     </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B26" t="s">
+        <v>245</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D26" t="s">
+        <v>243</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2291,7 +2319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CFD9C0-D986-A445-9050-436C9C79EAED}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -3015,8 +3043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1470E79-0876-1443-9948-BFC97695843C}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3415,18 +3443,8 @@
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="B26" t="s">
-        <v>245</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="D26" t="s">
-        <v>243</v>
-      </c>
+      <c r="A26" s="3"/>
+      <c r="C26" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>